<commit_message>
Renomeação de arquivos por processo
Renomeei alguns arquivos para que reflitam o processo correspondente, a saber: i) Carga fixa em xlsx; ii) Carga fracionada em pdf; iii) Carga fracionada em xlsx (PENDENTE), e; iv) Coverage (fluxo está na carga fixa em xlsx).
</commit_message>
<xml_diff>
--- a/pdf_location.xlsx
+++ b/pdf_location.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BlueShift075\Documents\GitHub\Intelipost-Media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{166E8B5E-35F0-4A12-B0DE-32E31EFFC703}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36"/>
+  <xr:revisionPtr documentId="13_ncr:1_{A0041D82-8512-40B2-AA9C-EF2E9E240796}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36"/>
   <bookViews>
     <workbookView windowHeight="8250" windowWidth="19200" xWindow="0" xr2:uid="{7B5AED11-F501-4C92-AA43-DD9CA8E6A848}" yWindow="0"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>PDF_LOC</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>C:\Users\BlueShift075\Documents\GitHub\Intelipost-Media\data-raw\cliente-eb\55004_PROPOSTA - EB - 28.02.19.pdf</t>
   </si>
@@ -390,7 +387,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>PDF_LOC</t>
+          <t>C:\Users\BlueShift075\Documents\GitHub\Intelipost-Media\data-raw\cliente-eb\55004_PROPOSTA - EB - 28.02.19.pdf</t>
         </is>
       </c>
     </row>

</xml_diff>